<commit_message>
1.22 gammma01 data, g02,03 exe HOME
</commit_message>
<xml_diff>
--- a/figure/FFN/FFN.xlsx
+++ b/figure/FFN/FFN.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\astrocyte_neuron\figure\FFN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B7E0BB7-6CF8-4D4F-BE1D-A7438C36ABC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98576F96-9AC4-4A1B-9E14-5CB2752A60A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="996" yWindow="4164" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="996" yWindow="4020" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -414,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -744,7 +743,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
@@ -767,7 +766,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>0.1</v>
       </c>
@@ -790,7 +789,7 @@
         <v>0.68489999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>0.2</v>
       </c>
@@ -813,7 +812,7 @@
         <v>0.65049999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>0.3</v>
       </c>
@@ -836,7 +835,7 @@
         <v>0.62309999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="2" t="s">
         <v>7</v>
@@ -847,7 +846,7 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
@@ -875,8 +874,23 @@
       <c r="I22" s="4">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="K22" s="9">
+        <v>2.6</v>
+      </c>
+      <c r="L22" s="9">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M22" s="9">
+        <v>4.5</v>
+      </c>
+      <c r="N22" s="9">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>0.1</v>
       </c>
@@ -904,8 +918,23 @@
       <c r="I23" s="6">
         <v>0.83689999999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>0.81430000000000002</v>
+      </c>
+      <c r="K23">
+        <v>0.83050000000000002</v>
+      </c>
+      <c r="L23">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="M23">
+        <v>0.75249999999999995</v>
+      </c>
+      <c r="N23">
+        <v>0.75070000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>0.2</v>
       </c>
@@ -925,7 +954,7 @@
         <v>0.85560000000000003</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>0.84030000000000005</v>
       </c>
       <c r="H24" s="6">
         <v>1</v>
@@ -934,7 +963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>0.3</v>
       </c>

</xml_diff>

<commit_message>
resort astro, add excel, rename folder, 2.8 MAC
</commit_message>
<xml_diff>
--- a/figure/FFN/FFN.xlsx
+++ b/figure/FFN/FFN.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\astrocyte_neuron\figure\FFN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dodo/astrocyte_neuron/figure/FFN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98576F96-9AC4-4A1B-9E14-5CB2752A60A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E7F955-45A9-F441-BF60-F8A35004AD48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="996" yWindow="4020" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
   <si>
     <t>纯GABA (p=0)</t>
   </si>
@@ -44,13 +46,224 @@
   </si>
   <si>
     <t>纯AMPA p=1</t>
+  </si>
+  <si>
+    <t>gamma</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>波浪</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>波类型</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPAD150单中心稳定螺旋波</t>
+  </si>
+  <si>
+    <t>波浪虫眼</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPAD250扩散阴阳螺旋波</t>
+  </si>
+  <si>
+    <t>AMPAD260扩散阴阳螺旋波</t>
+  </si>
+  <si>
+    <t>扩散波</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>同步</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>双心螺旋波</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPAD320螺旋波变化极慢</t>
+  </si>
+  <si>
+    <t>AMPAD330嵌套螺旋波</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPAD340单中心稳定螺旋波</t>
+  </si>
+  <si>
+    <t>AMPAD400扩散螺旋波</t>
+  </si>
+  <si>
+    <t>AMPAD420四角螺旋波</t>
+  </si>
+  <si>
+    <t>AMPAD430四角螺旋波</t>
+  </si>
+  <si>
+    <t>AMPAD440四角螺旋波</t>
+  </si>
+  <si>
+    <t>AMPAD450四角螺旋波</t>
+  </si>
+  <si>
+    <t>AMPAD460特别扩散螺旋波</t>
+  </si>
+  <si>
+    <t>混乱</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPAD030破碎螺旋波</t>
+  </si>
+  <si>
+    <t>AMPAD050单中心稳定螺旋波</t>
+  </si>
+  <si>
+    <t>AMPAD030破碎螺旋波</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPAD050破碎螺旋波</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>周围破碎迁移螺旋波</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPAD070单中心稳定螺旋波</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPAD080单中心稳定螺旋波</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPAD090不稳定方形靶波</t>
+  </si>
+  <si>
+    <t>AMPAD110不稳定方形靶波</t>
+  </si>
+  <si>
+    <t>AMPAD120不稳定方形靶波</t>
+  </si>
+  <si>
+    <t>AMPAD130不稳定靶波过渡</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPAD140转变messy</t>
+  </si>
+  <si>
+    <t>messy</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>不稳定中心靶波</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>成型messy过渡</t>
+  </si>
+  <si>
+    <t>成型messy过渡</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>不稳定中心靶波合并</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>不稳定中心靶波螺旋波交变</t>
+  </si>
+  <si>
+    <t>AMPAD370双中心螺旋波吞并</t>
+  </si>
+  <si>
+    <t>AMPAD400双中心靶波稳定存在</t>
+  </si>
+  <si>
+    <t>AMPAD420双中心螺旋波稳定存在</t>
+  </si>
+  <si>
+    <t>AMPAD030_多中心螺旋波_7w步后变化慢</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPAD050中心缺陷螺旋波</t>
+  </si>
+  <si>
+    <t>AMPAD080双心螺旋波</t>
+  </si>
+  <si>
+    <t>不成形大靶波</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>过渡messy</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>不稳定中心螺旋波</t>
+  </si>
+  <si>
+    <t>多中心螺旋波吞并静止</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>多中心螺旋波吞并</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPAD450双中心稳定螺旋波</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPAD450双中心稳定螺旋波吞并ing</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>波浪（靶波）</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">gamma </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPAD060中心破碎螺旋波</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPAD070中心破碎螺旋波</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>中心破碎螺旋波扩散</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPAD370多中心稳定螺旋波</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPAD350双中心螺旋波吞并</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,8 +284,46 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -82,6 +333,60 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -127,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -138,6 +443,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -412,22 +740,1144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9309CA5-B4FD-044A-B7EF-9F9B6F26A726}">
+  <dimension ref="A1:G48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
+    <col min="7" max="7" width="30.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="C2">
+        <v>0.2</v>
+      </c>
+      <c r="D2">
+        <v>0.3</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="F2">
+        <v>0.2</v>
+      </c>
+      <c r="G2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>0.1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>0.2</v>
+      </c>
+      <c r="B4">
+        <v>0.995</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>0.3</v>
+      </c>
+      <c r="B5">
+        <v>0.93620000000000003</v>
+      </c>
+      <c r="C5">
+        <v>0.95009999999999994</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.97609999999999997</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>0.4</v>
+      </c>
+      <c r="F6" s="16"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>0.5</v>
+      </c>
+      <c r="B7">
+        <v>0.8962</v>
+      </c>
+      <c r="C7">
+        <v>0.89990000000000003</v>
+      </c>
+      <c r="D7">
+        <v>0.91090000000000004</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>0.6</v>
+      </c>
+      <c r="B8">
+        <v>0.88419999999999999</v>
+      </c>
+      <c r="C8">
+        <v>0.85140000000000005</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>0.7</v>
+      </c>
+      <c r="B9">
+        <v>0.89559999999999995</v>
+      </c>
+      <c r="C9">
+        <v>0.8669</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>0.8</v>
+      </c>
+      <c r="B10">
+        <v>0.88629999999999998</v>
+      </c>
+      <c r="C10">
+        <v>0.8599</v>
+      </c>
+      <c r="D10">
+        <v>0.8589</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>0.9</v>
+      </c>
+      <c r="B11">
+        <v>0.87760000000000005</v>
+      </c>
+      <c r="C11">
+        <v>0.871</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>0.85589999999999999</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B13">
+        <v>0.87619999999999998</v>
+      </c>
+      <c r="C13">
+        <v>0.85450000000000004</v>
+      </c>
+      <c r="D13">
+        <v>0.86529999999999996</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>1.2</v>
+      </c>
+      <c r="B14">
+        <v>0.88690000000000002</v>
+      </c>
+      <c r="C14">
+        <v>0.85150000000000003</v>
+      </c>
+      <c r="D14">
+        <v>0.85580000000000001</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>1.3</v>
+      </c>
+      <c r="B15">
+        <v>0.87619999999999998</v>
+      </c>
+      <c r="C15">
+        <v>0.84850000000000003</v>
+      </c>
+      <c r="D15">
+        <v>0.8458</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>1.4</v>
+      </c>
+      <c r="B16">
+        <v>0.871</v>
+      </c>
+      <c r="C16">
+        <v>0.89410000000000001</v>
+      </c>
+      <c r="D16">
+        <v>0.83889999999999998</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>1.5</v>
+      </c>
+      <c r="B17">
+        <v>0.83679999999999999</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>1.6</v>
+      </c>
+      <c r="B18">
+        <v>0.86170000000000002</v>
+      </c>
+      <c r="C18">
+        <v>0.86619999999999997</v>
+      </c>
+      <c r="D18">
+        <v>0.82520000000000004</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>1.7</v>
+      </c>
+      <c r="B19">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="C19">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="D19">
+        <v>0.80959999999999999</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>1.8</v>
+      </c>
+      <c r="B20">
+        <v>0.83730000000000004</v>
+      </c>
+      <c r="C20">
+        <v>0.83530000000000004</v>
+      </c>
+      <c r="D20">
+        <v>0.80330000000000001</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>1.9</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>0.79730000000000001</v>
+      </c>
+      <c r="C22">
+        <v>0.80659999999999998</v>
+      </c>
+      <c r="D22">
+        <v>0.79220000000000002</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>2.1</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B24">
+        <v>0.78549999999999998</v>
+      </c>
+      <c r="C24">
+        <v>0.78380000000000005</v>
+      </c>
+      <c r="D24">
+        <v>0.76419999999999999</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B25">
+        <v>0.78910000000000002</v>
+      </c>
+      <c r="C25">
+        <v>0.77280000000000004</v>
+      </c>
+      <c r="D25">
+        <v>0.75109999999999999</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>2.4</v>
+      </c>
+      <c r="B26">
+        <v>0.81089999999999995</v>
+      </c>
+      <c r="C26">
+        <v>0.76119999999999999</v>
+      </c>
+      <c r="D26">
+        <v>0.74060000000000004</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>2.5</v>
+      </c>
+      <c r="B27">
+        <v>0.81430000000000002</v>
+      </c>
+      <c r="C27">
+        <v>0.75190000000000001</v>
+      </c>
+      <c r="D27">
+        <v>0.72929999999999995</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>2.6</v>
+      </c>
+      <c r="B28">
+        <v>0.83050000000000002</v>
+      </c>
+      <c r="C28">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>2.7</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>2.8</v>
+      </c>
+      <c r="B30">
+        <v>0.85029999999999994</v>
+      </c>
+      <c r="C30">
+        <v>0.74680000000000002</v>
+      </c>
+      <c r="D30">
+        <v>0.71120000000000005</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>2.9</v>
+      </c>
+      <c r="B31">
+        <v>0.84719999999999995</v>
+      </c>
+      <c r="C31">
+        <v>0.75270000000000004</v>
+      </c>
+      <c r="D31">
+        <v>0.69610000000000005</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>0.77380000000000004</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <v>3.1</v>
+      </c>
+      <c r="G33" s="19"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <v>3.2</v>
+      </c>
+      <c r="B34">
+        <v>0.82320000000000004</v>
+      </c>
+      <c r="C34">
+        <v>0.75349999999999995</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <v>3.3</v>
+      </c>
+      <c r="B35">
+        <v>0.81410000000000005</v>
+      </c>
+      <c r="C35">
+        <v>0.78190000000000004</v>
+      </c>
+      <c r="D35">
+        <v>0.70679999999999998</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G35" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <v>3.4</v>
+      </c>
+      <c r="B36">
+        <v>0.80479999999999996</v>
+      </c>
+      <c r="C36">
+        <v>0.77580000000000005</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
+        <v>3.5</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>0.79790000000000005</v>
+      </c>
+      <c r="D37">
+        <v>0.71419999999999995</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
+        <v>3.6</v>
+      </c>
+      <c r="F38" s="29"/>
+      <c r="G38" s="21"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39">
+        <v>3.7</v>
+      </c>
+      <c r="B39">
+        <v>0.78110000000000002</v>
+      </c>
+      <c r="C39">
+        <v>0.755</v>
+      </c>
+      <c r="D39">
+        <v>0.73170000000000002</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" s="21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40">
+        <v>3.8</v>
+      </c>
+      <c r="E40" s="11"/>
+      <c r="F40" s="29"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41">
+        <v>3.9</v>
+      </c>
+      <c r="E41" s="11"/>
+      <c r="F41" s="29"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>0.77159999999999995</v>
+      </c>
+      <c r="C42">
+        <v>0.78810000000000002</v>
+      </c>
+      <c r="D42">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="G42" s="21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44">
+        <v>4.2</v>
+      </c>
+      <c r="B44">
+        <v>0.76370000000000005</v>
+      </c>
+      <c r="C44">
+        <v>0.77590000000000003</v>
+      </c>
+      <c r="D44">
+        <v>0.70289999999999997</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45">
+        <v>4.3</v>
+      </c>
+      <c r="B45">
+        <v>0.75890000000000002</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>0.67379999999999995</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B46">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>0.66969999999999996</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47">
+        <v>4.5</v>
+      </c>
+      <c r="B47">
+        <v>0.75249999999999995</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B48">
+        <v>0.75070000000000003</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>0.7097</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E13B5C-7F0A-DF4A-90E4-ECDD36DEDEBD}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>0.1</v>
+      </c>
+      <c r="C2">
+        <v>0.2</v>
+      </c>
+      <c r="D2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>0.25</v>
+      </c>
+      <c r="B6">
+        <v>0.96109999999999995</v>
+      </c>
+      <c r="C6">
+        <v>0.98340000000000005</v>
+      </c>
+      <c r="D6">
+        <v>0.97009999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>0.3</v>
+      </c>
+      <c r="B7">
+        <v>0.94189999999999996</v>
+      </c>
+      <c r="C7">
+        <v>0.99270000000000003</v>
+      </c>
+      <c r="D7">
+        <v>0.99550000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>0.35</v>
+      </c>
+      <c r="B8">
+        <v>0.91569999999999996</v>
+      </c>
+      <c r="C8">
+        <v>0.91279999999999994</v>
+      </c>
+      <c r="D8">
+        <v>0.9123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>0.4</v>
+      </c>
+      <c r="B9">
+        <v>0.871</v>
+      </c>
+      <c r="C9">
+        <v>0.87929999999999997</v>
+      </c>
+      <c r="D9">
+        <v>0.88349999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>0.45</v>
+      </c>
+      <c r="B10">
+        <v>0.80589999999999995</v>
+      </c>
+      <c r="C10">
+        <v>0.79220000000000002</v>
+      </c>
+      <c r="D10">
+        <v>0.81299999999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>0.5</v>
+      </c>
+      <c r="B11">
+        <v>0.77549999999999997</v>
+      </c>
+      <c r="C11">
+        <v>0.8609</v>
+      </c>
+      <c r="D11">
+        <v>0.9496</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B12">
+        <v>0.75049999999999994</v>
+      </c>
+      <c r="C12">
+        <v>0.72440000000000004</v>
+      </c>
+      <c r="D12">
+        <v>0.69530000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -450,7 +1900,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="5">
         <v>0.1</v>
       </c>
@@ -473,7 +1923,7 @@
         <v>0.43719999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="5">
         <v>0.2</v>
       </c>
@@ -496,7 +1946,7 @@
         <v>0.502</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="5">
         <v>0.3</v>
       </c>
@@ -520,7 +1970,7 @@
       </c>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="5"/>
       <c r="B6" s="2" t="s">
         <v>2</v>
@@ -533,7 +1983,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -556,7 +2006,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="5">
         <v>0.1</v>
       </c>
@@ -579,7 +2029,7 @@
         <v>0.59760000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="5">
         <v>0.2</v>
       </c>
@@ -602,7 +2052,7 @@
         <v>0.5827</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="5">
         <v>0.3</v>
       </c>
@@ -625,7 +2075,7 @@
         <v>0.57320000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="5"/>
       <c r="B11" s="2" t="s">
         <v>4</v>
@@ -638,7 +2088,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
@@ -661,7 +2111,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="5">
         <v>0.1</v>
       </c>
@@ -684,7 +2134,7 @@
         <v>0.63980000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="5">
         <v>0.2</v>
       </c>
@@ -707,7 +2157,7 @@
         <v>0.61099999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="5">
         <v>0.3</v>
       </c>
@@ -730,7 +2180,7 @@
         <v>0.5907</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="5"/>
       <c r="B16" s="2" t="s">
         <v>5</v>
@@ -743,7 +2193,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
@@ -766,7 +2216,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" s="5">
         <v>0.1</v>
       </c>
@@ -789,7 +2239,7 @@
         <v>0.68489999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="A19" s="5">
         <v>0.2</v>
       </c>
@@ -812,7 +2262,7 @@
         <v>0.65049999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" s="5">
         <v>0.3</v>
       </c>
@@ -835,7 +2285,7 @@
         <v>0.62309999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" s="5"/>
       <c r="B21" s="2" t="s">
         <v>7</v>
@@ -846,7 +2296,7 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
@@ -890,7 +2340,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="5">
         <v>0.1</v>
       </c>
@@ -934,7 +2384,7 @@
         <v>0.75070000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="A24" s="5">
         <v>0.2</v>
       </c>
@@ -963,7 +2413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="A25" s="5">
         <v>0.3</v>
       </c>

</xml_diff>

<commit_message>
2.8 Origin FFN HOME
</commit_message>
<xml_diff>
--- a/figure/FFN/FFN.xlsx
+++ b/figure/FFN/FFN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dodo/astrocyte_neuron/figure/FFN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\astrocyte_neuron\figure\FFN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E7F955-45A9-F441-BF60-F8A35004AD48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B07D5AD-CCBA-41AE-91A2-6F99242B2C35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1500" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -263,7 +263,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -448,7 +448,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -456,9 +455,6 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -466,6 +462,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -741,30 +740,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9309CA5-B4FD-044A-B7EF-9F9B6F26A726}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="133" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="27" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
     <col min="7" max="7" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="23" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
@@ -787,7 +786,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.1</v>
       </c>
@@ -800,17 +799,17 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.2</v>
       </c>
@@ -823,17 +822,17 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.3</v>
       </c>
@@ -846,23 +845,32 @@
       <c r="D5" s="10">
         <v>0.97609999999999997</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>31</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.4</v>
       </c>
-      <c r="F6" s="16"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="B6">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="C6">
+        <v>0.91759999999999997</v>
+      </c>
+      <c r="D6">
+        <v>0.9698</v>
+      </c>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -878,14 +886,14 @@
       <c r="E7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.6</v>
       </c>
@@ -898,17 +906,17 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="22" t="s">
         <v>62</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.7</v>
       </c>
@@ -921,17 +929,17 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="22" t="s">
         <v>63</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.8</v>
       </c>
@@ -944,7 +952,7 @@
       <c r="D10">
         <v>0.8589</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="22" t="s">
         <v>64</v>
       </c>
       <c r="F10" s="13" t="s">
@@ -954,7 +962,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.9</v>
       </c>
@@ -967,17 +975,17 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -990,17 +998,17 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1.1000000000000001</v>
       </c>
@@ -1016,14 +1024,14 @@
       <c r="E13" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.2</v>
       </c>
@@ -1039,14 +1047,14 @@
       <c r="E14" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="27" t="s">
+      <c r="G14" s="25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.3</v>
       </c>
@@ -1062,14 +1070,14 @@
       <c r="E15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1.4</v>
       </c>
@@ -1085,14 +1093,14 @@
       <c r="E16" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.5</v>
       </c>
@@ -1108,14 +1116,14 @@
       <c r="E17" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="26" t="s">
+      <c r="G17" s="24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.6</v>
       </c>
@@ -1134,11 +1142,11 @@
       <c r="F18" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="27" t="s">
+      <c r="G18" s="25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.7</v>
       </c>
@@ -1157,11 +1165,11 @@
       <c r="F19" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="27" t="s">
+      <c r="G19" s="25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1.8</v>
       </c>
@@ -1180,29 +1188,45 @@
       <c r="F20" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1.9</v>
-      </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="14"/>
-    </row>
-    <row r="22" spans="1:7">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>0.79730000000000001</v>
+      </c>
+      <c r="C21">
+        <v>0.80659999999999998</v>
+      </c>
+      <c r="D21">
+        <v>0.79220000000000002</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B22">
-        <v>0.79730000000000001</v>
+        <v>0.78549999999999998</v>
       </c>
       <c r="C22">
-        <v>0.80659999999999998</v>
+        <v>0.78380000000000005</v>
       </c>
       <c r="D22">
-        <v>0.79220000000000002</v>
+        <v>0.76419999999999999</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>60</v>
@@ -1214,29 +1238,44 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2.1</v>
-      </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="15"/>
-    </row>
-    <row r="24" spans="1:7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B23">
+        <v>0.78910000000000002</v>
+      </c>
+      <c r="C23">
+        <v>0.77280000000000004</v>
+      </c>
+      <c r="D23">
+        <v>0.75109999999999999</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2.2000000000000002</v>
+        <v>2.4</v>
       </c>
       <c r="B24">
-        <v>0.78549999999999998</v>
+        <v>0.81089999999999995</v>
       </c>
       <c r="C24">
-        <v>0.78380000000000005</v>
+        <v>0.76119999999999999</v>
       </c>
       <c r="D24">
-        <v>0.76419999999999999</v>
+        <v>0.74060000000000004</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="F24" s="14" t="s">
         <v>41</v>
@@ -1245,460 +1284,453 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2.2999999999999998</v>
+        <v>2.5</v>
       </c>
       <c r="B25">
-        <v>0.78910000000000002</v>
+        <v>0.81430000000000002</v>
       </c>
       <c r="C25">
-        <v>0.77280000000000004</v>
+        <v>0.75190000000000001</v>
       </c>
       <c r="D25">
-        <v>0.75109999999999999</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>41</v>
+        <v>0.72929999999999995</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="G25" s="14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2.4</v>
+        <v>2.6</v>
       </c>
       <c r="B26">
-        <v>0.81089999999999995</v>
+        <v>0.83050000000000002</v>
       </c>
       <c r="C26">
-        <v>0.76119999999999999</v>
+        <v>0.74099999999999999</v>
       </c>
       <c r="D26">
-        <v>0.74060000000000004</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>41</v>
+        <v>1</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="G26" s="14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2.5</v>
+        <v>2.8</v>
       </c>
       <c r="B27">
-        <v>0.81430000000000002</v>
+        <v>0.85029999999999994</v>
       </c>
       <c r="C27">
-        <v>0.75190000000000001</v>
+        <v>0.74680000000000002</v>
       </c>
       <c r="D27">
-        <v>0.72929999999999995</v>
-      </c>
-      <c r="E27" s="28" t="s">
-        <v>14</v>
+        <v>0.71120000000000005</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G27" s="14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2.6</v>
+        <v>2.9</v>
       </c>
       <c r="B28">
-        <v>0.83050000000000002</v>
+        <v>0.84719999999999995</v>
       </c>
       <c r="C28">
-        <v>0.74099999999999999</v>
+        <v>0.75270000000000004</v>
       </c>
       <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>15</v>
+        <v>0.69610000000000005</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G28" s="14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2.7</v>
-      </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0.77380000000000004</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2.8</v>
+        <v>3.1</v>
       </c>
       <c r="B30">
-        <v>0.85029999999999994</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>0.74680000000000002</v>
+        <v>0.80049999999999999</v>
       </c>
       <c r="D30">
-        <v>0.71120000000000005</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>0.69310000000000005</v>
+      </c>
+      <c r="G30" s="18"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2.9</v>
+        <v>3.2</v>
       </c>
       <c r="B31">
-        <v>0.84719999999999995</v>
+        <v>0.82320000000000004</v>
       </c>
       <c r="C31">
-        <v>0.75270000000000004</v>
+        <v>0.75349999999999995</v>
       </c>
       <c r="D31">
-        <v>0.69610000000000005</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>0.81410000000000005</v>
       </c>
       <c r="C32">
-        <v>0.77380000000000004</v>
+        <v>0.78190000000000004</v>
       </c>
       <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" s="19" t="s">
+        <v>0.70679999999999998</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G32" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3.4</v>
+      </c>
+      <c r="B33">
+        <v>0.80479999999999996</v>
+      </c>
+      <c r="C33">
+        <v>0.77580000000000005</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G33" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="G32" s="19" t="s">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>3.5</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>0.79790000000000005</v>
+      </c>
+      <c r="D34">
+        <v>0.71419999999999995</v>
+      </c>
+      <c r="E34" s="18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33">
-        <v>3.1</v>
-      </c>
-      <c r="G33" s="19"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34">
-        <v>3.2</v>
-      </c>
-      <c r="B34">
-        <v>0.82320000000000004</v>
-      </c>
-      <c r="C34">
-        <v>0.75349999999999995</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" s="20" t="s">
+      <c r="F34" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="G34" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G34" s="19" t="s">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>3.6</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0.80449999999999999</v>
+      </c>
+      <c r="D35" s="11">
+        <v>0.69240000000000002</v>
+      </c>
+      <c r="E35" s="18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35">
-        <v>3.3</v>
-      </c>
-      <c r="B35">
-        <v>0.81410000000000005</v>
-      </c>
-      <c r="C35">
-        <v>0.78190000000000004</v>
-      </c>
-      <c r="D35">
-        <v>0.70679999999999998</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="G35" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="F35" s="27"/>
+      <c r="G35" s="20"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="B36">
-        <v>0.80479999999999996</v>
+        <v>0.78110000000000002</v>
       </c>
       <c r="C36">
-        <v>0.77580000000000005</v>
+        <v>0.755</v>
       </c>
       <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="G36" s="19" t="s">
+        <v>0.73170000000000002</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>3.8</v>
+      </c>
+      <c r="B37">
+        <v>0.77790000000000004</v>
+      </c>
+      <c r="C37">
+        <v>0.80289999999999995</v>
+      </c>
+      <c r="D37" s="11">
+        <v>0.71379999999999999</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="27"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>3.9</v>
+      </c>
+      <c r="B38">
+        <v>0.77490000000000003</v>
+      </c>
+      <c r="C38" s="11">
+        <v>0.78149999999999997</v>
+      </c>
+      <c r="D38" s="11">
+        <v>0.70920000000000005</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="F38" s="27"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <v>0.77159999999999995</v>
+      </c>
+      <c r="C39">
+        <v>0.78810000000000002</v>
+      </c>
+      <c r="D39">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B40">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="C40">
+        <v>0.78039999999999998</v>
+      </c>
+      <c r="D40">
+        <v>0.70350000000000001</v>
+      </c>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>4.2</v>
+      </c>
+      <c r="B41">
+        <v>0.76370000000000005</v>
+      </c>
+      <c r="C41">
+        <v>0.77590000000000003</v>
+      </c>
+      <c r="D41">
+        <v>0.70289999999999997</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>4.3</v>
+      </c>
+      <c r="B42">
+        <v>0.75890000000000002</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>0.67379999999999995</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" s="18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37">
-        <v>3.5</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37">
-        <v>0.79790000000000005</v>
-      </c>
-      <c r="D37">
-        <v>0.71419999999999995</v>
-      </c>
-      <c r="E37" s="19" t="s">
+      <c r="G42" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B43">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>0.66969999999999996</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38">
-        <v>3.6</v>
-      </c>
-      <c r="F38" s="29"/>
-      <c r="G38" s="21"/>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39">
-        <v>3.7</v>
-      </c>
-      <c r="B39">
-        <v>0.78110000000000002</v>
-      </c>
-      <c r="C39">
-        <v>0.755</v>
-      </c>
-      <c r="D39">
-        <v>0.73170000000000002</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F39" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="G39" s="21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40">
-        <v>3.8</v>
-      </c>
-      <c r="E40" s="11"/>
-      <c r="F40" s="29"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41">
-        <v>3.9</v>
-      </c>
-      <c r="E41" s="11"/>
-      <c r="F41" s="29"/>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42">
-        <v>4</v>
-      </c>
-      <c r="B42">
-        <v>0.77159999999999995</v>
-      </c>
-      <c r="C42">
-        <v>0.78810000000000002</v>
-      </c>
-      <c r="D42">
-        <v>0.71250000000000002</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F42" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="G42" s="21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="G43" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="B44">
-        <v>0.76370000000000005</v>
+        <v>0.75249999999999995</v>
       </c>
       <c r="C44">
-        <v>0.77590000000000003</v>
+        <v>1</v>
       </c>
       <c r="D44">
-        <v>0.70289999999999997</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>49</v>
+        <v>26</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>4.3</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="B45">
-        <v>0.75890000000000002</v>
+        <v>0.75070000000000003</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45">
-        <v>0.67379999999999995</v>
+        <v>0.7097</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F45" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" s="18" t="s">
         <v>17</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="B46">
-        <v>0.75600000000000001</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46">
-        <v>0.66969999999999996</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F46" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G46" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47">
-        <v>4.5</v>
-      </c>
-      <c r="B47">
-        <v>0.75249999999999995</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47">
-        <v>0.71199999999999997</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F47" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="B48">
-        <v>0.75070000000000003</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-      <c r="D48">
-        <v>0.7097</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F48" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G48" s="12" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1708,7 +1740,7 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1720,15 +1752,15 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
@@ -1742,22 +1774,22 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.25</v>
       </c>
@@ -1771,7 +1803,7 @@
         <v>0.97009999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.3</v>
       </c>
@@ -1785,7 +1817,7 @@
         <v>0.99550000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.35</v>
       </c>
@@ -1799,7 +1831,7 @@
         <v>0.9123</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.4</v>
       </c>
@@ -1813,7 +1845,7 @@
         <v>0.88349999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.45</v>
       </c>
@@ -1827,7 +1859,7 @@
         <v>0.81299999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.5</v>
       </c>
@@ -1841,7 +1873,7 @@
         <v>0.9496</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.55000000000000004</v>
       </c>
@@ -1869,15 +1901,15 @@
       <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1900,7 +1932,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>0.1</v>
       </c>
@@ -1923,7 +1955,7 @@
         <v>0.43719999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>0.2</v>
       </c>
@@ -1946,7 +1978,7 @@
         <v>0.502</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>0.3</v>
       </c>
@@ -1970,7 +2002,7 @@
       </c>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="2" t="s">
         <v>2</v>
@@ -1983,7 +2015,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -2006,7 +2038,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>0.1</v>
       </c>
@@ -2029,7 +2061,7 @@
         <v>0.59760000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>0.2</v>
       </c>
@@ -2052,7 +2084,7 @@
         <v>0.5827</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>0.3</v>
       </c>
@@ -2075,7 +2107,7 @@
         <v>0.57320000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="2" t="s">
         <v>4</v>
@@ -2088,7 +2120,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
@@ -2111,7 +2143,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>0.1</v>
       </c>
@@ -2134,7 +2166,7 @@
         <v>0.63980000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>0.2</v>
       </c>
@@ -2157,7 +2189,7 @@
         <v>0.61099999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>0.3</v>
       </c>
@@ -2180,7 +2212,7 @@
         <v>0.5907</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="2" t="s">
         <v>5</v>
@@ -2193,7 +2225,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
@@ -2216,7 +2248,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>0.1</v>
       </c>
@@ -2239,7 +2271,7 @@
         <v>0.68489999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>0.2</v>
       </c>
@@ -2262,7 +2294,7 @@
         <v>0.65049999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>0.3</v>
       </c>
@@ -2285,7 +2317,7 @@
         <v>0.62309999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="2" t="s">
         <v>7</v>
@@ -2296,7 +2328,7 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
@@ -2340,7 +2372,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>0.1</v>
       </c>
@@ -2384,7 +2416,7 @@
         <v>0.75070000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>0.2</v>
       </c>
@@ -2413,7 +2445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>0.3</v>
       </c>

</xml_diff>

<commit_message>
2.18 FFN obj HOME
</commit_message>
<xml_diff>
--- a/figure/FFN/FFN.xlsx
+++ b/figure/FFN/FFN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\astrocyte_neuron\figure\FFN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765C74D3-6C01-4968-B96F-F29435ECB9AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0913529-ABA0-492B-8C5F-66ABF1AF35B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8952" yWindow="1800" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="3744" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -402,14 +402,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -687,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9309CA5-B4FD-044A-B7EF-9F9B6F26A726}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="133" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -942,7 +942,7 @@
       <c r="A12">
         <v>1</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="23">
         <v>0.85589999999999999</v>
       </c>
       <c r="C12">
@@ -1046,7 +1046,7 @@
       <c r="E16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="25" t="s">
         <v>32</v>
       </c>
       <c r="G16" s="21" t="s">
@@ -1058,18 +1058,18 @@
         <v>1.5</v>
       </c>
       <c r="B17" s="11">
-        <v>0.83679999999999999</v>
+        <v>0.86629999999999996</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0.88</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0.83260000000000001</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="27" t="s">
         <v>16</v>
       </c>
       <c r="G17" s="20" t="s">
@@ -1089,7 +1089,7 @@
       <c r="D18">
         <v>0.82520000000000004</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="18" t="s">
         <v>49</v>
       </c>
       <c r="F18" s="13" t="s">
@@ -1112,7 +1112,7 @@
       <c r="D19">
         <v>0.80959999999999999</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="18" t="s">
         <v>49</v>
       </c>
       <c r="F19" s="13" t="s">
@@ -1135,7 +1135,7 @@
       <c r="D20">
         <v>0.80330000000000001</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="18" t="s">
         <v>49</v>
       </c>
       <c r="F20" s="13" t="s">
@@ -1158,7 +1158,7 @@
       <c r="D21">
         <v>0.79220000000000002</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="18" t="s">
         <v>49</v>
       </c>
       <c r="F21" s="13" t="s">
@@ -1181,7 +1181,7 @@
       <c r="D22" s="11">
         <v>0.76419999999999999</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="18" t="s">
         <v>49</v>
       </c>
       <c r="F22" s="13" t="s">
@@ -1204,7 +1204,7 @@
       <c r="D23">
         <v>0.75109999999999999</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="18" t="s">
         <v>49</v>
       </c>
       <c r="F23" s="13" t="s">
@@ -1227,7 +1227,7 @@
       <c r="D24">
         <v>0.74060000000000004</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="18" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="13" t="s">
@@ -1250,10 +1250,10 @@
       <c r="D25">
         <v>0.72929999999999995</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E25" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="13" t="s">
         <v>36</v>
       </c>
       <c r="G25" s="13" t="s">
@@ -1273,10 +1273,10 @@
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="E26" s="22" t="s">
+      <c r="E26" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="25" t="s">
         <v>35</v>
       </c>
       <c r="G26" s="13" t="s">
@@ -1299,7 +1299,7 @@
       <c r="E27" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F27" s="25" t="s">
         <v>35</v>
       </c>
       <c r="G27" s="13" t="s">
@@ -1371,7 +1371,7 @@
       <c r="F30" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="17" t="s">
+      <c r="G30" s="25" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1460,7 +1460,7 @@
       <c r="E34" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="23" t="s">
+      <c r="F34" s="22" t="s">
         <v>52</v>
       </c>
       <c r="G34" s="16" t="s">
@@ -1477,13 +1477,13 @@
       <c r="C35">
         <v>0.80449999999999999</v>
       </c>
-      <c r="D35" s="24">
+      <c r="D35" s="23">
         <v>0.69240000000000002</v>
       </c>
       <c r="E35" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F35" s="23" t="s">
+      <c r="F35" s="22" t="s">
         <v>53</v>
       </c>
       <c r="G35" s="16" t="s">
@@ -1506,7 +1506,7 @@
       <c r="E36" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F36" s="23" t="s">
+      <c r="F36" s="22" t="s">
         <v>39</v>
       </c>
       <c r="G36" s="17" t="s">
@@ -1529,10 +1529,10 @@
       <c r="E37" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F37" s="23" t="s">
+      <c r="F37" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="G37" s="25" t="s">
+      <c r="G37" s="24" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1552,10 +1552,10 @@
       <c r="E38" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F38" s="23" t="s">
+      <c r="F38" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="G38" s="25" t="s">
+      <c r="G38" s="24" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1575,10 +1575,10 @@
       <c r="E39" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F39" s="23" t="s">
+      <c r="F39" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G39" s="17" t="s">
+      <c r="G39" s="11" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1598,10 +1598,10 @@
       <c r="E40" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F40" s="25" t="s">
+      <c r="F40" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="G40" s="23" t="s">
+      <c r="G40" s="22" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update FFN excel HOME
</commit_message>
<xml_diff>
--- a/figure/FFN/FFN.xlsx
+++ b/figure/FFN/FFN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\astrocyte_neuron\figure\FFN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0913529-ABA0-492B-8C5F-66ABF1AF35B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE40227D-C0ED-4A15-A564-9C3E4CEFE0DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="3744" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="3372" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -406,10 +406,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -688,7 +688,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -699,11 +699,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="10" t="s">
         <v>10</v>
       </c>
@@ -851,7 +851,7 @@
         <v>0.6</v>
       </c>
       <c r="B8">
-        <v>0.88419999999999999</v>
+        <v>0.85919999999999996</v>
       </c>
       <c r="C8">
         <v>0.88180000000000003</v>
@@ -1069,7 +1069,7 @@
       <c r="E17" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="26" t="s">
         <v>16</v>
       </c>
       <c r="G17" s="20" t="s">

</xml_diff>

<commit_message>
2.20 resort data HOME
</commit_message>
<xml_diff>
--- a/figure/FFN/FFN.xlsx
+++ b/figure/FFN/FFN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\astrocyte_neuron\figure\FFN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE40227D-C0ED-4A15-A564-9C3E4CEFE0DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936A8D5C-2BE9-4944-A3E4-8D0F807C074F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="3372" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -379,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -400,13 +400,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -687,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9309CA5-B4FD-044A-B7EF-9F9B6F26A726}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="133" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -699,11 +697,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="10" t="s">
         <v>10</v>
       </c>
@@ -942,7 +940,7 @@
       <c r="A12">
         <v>1</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="22">
         <v>0.85589999999999999</v>
       </c>
       <c r="C12">
@@ -980,7 +978,7 @@
       <c r="F13" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="20" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1003,7 +1001,7 @@
       <c r="F14" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="20" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1023,10 +1021,10 @@
       <c r="E15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="20" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1046,10 +1044,10 @@
       <c r="E16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="20" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1069,11 +1067,11 @@
       <c r="E17" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="26" t="s">
-        <v>16</v>
+      <c r="F17" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1095,7 +1093,7 @@
       <c r="F18" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="20" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1118,7 +1116,7 @@
       <c r="F19" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="G19" s="20" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1276,11 +1274,11 @@
       <c r="E26" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="25" t="s">
+      <c r="F26" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="G26" s="13" t="s">
-        <v>33</v>
+      <c r="G26" s="15" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1299,7 +1297,7 @@
       <c r="E27" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="25" t="s">
+      <c r="F27" s="24" t="s">
         <v>35</v>
       </c>
       <c r="G27" s="13" t="s">
@@ -1371,7 +1369,7 @@
       <c r="F30" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="25" t="s">
+      <c r="G30" s="24" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1460,7 +1458,7 @@
       <c r="E34" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="22" t="s">
+      <c r="F34" s="21" t="s">
         <v>52</v>
       </c>
       <c r="G34" s="16" t="s">
@@ -1477,13 +1475,13 @@
       <c r="C35">
         <v>0.80449999999999999</v>
       </c>
-      <c r="D35" s="23">
+      <c r="D35" s="22">
         <v>0.69240000000000002</v>
       </c>
       <c r="E35" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F35" s="22" t="s">
+      <c r="F35" s="21" t="s">
         <v>53</v>
       </c>
       <c r="G35" s="16" t="s">
@@ -1506,7 +1504,7 @@
       <c r="E36" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F36" s="22" t="s">
+      <c r="F36" s="21" t="s">
         <v>39</v>
       </c>
       <c r="G36" s="17" t="s">
@@ -1529,10 +1527,10 @@
       <c r="E37" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F37" s="22" t="s">
+      <c r="F37" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="G37" s="24" t="s">
+      <c r="G37" s="23" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1552,10 +1550,10 @@
       <c r="E38" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F38" s="22" t="s">
+      <c r="F38" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G38" s="24" t="s">
+      <c r="G38" s="23" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1575,7 +1573,7 @@
       <c r="E39" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F39" s="22" t="s">
+      <c r="F39" s="21" t="s">
         <v>40</v>
       </c>
       <c r="G39" s="11" t="s">
@@ -1598,10 +1596,10 @@
       <c r="E40" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F40" s="24" t="s">
+      <c r="F40" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="G40" s="22" t="s">
+      <c r="G40" s="21" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2.22 astro gamma0.4 init HOME
</commit_message>
<xml_diff>
--- a/figure/FFN/FFN.xlsx
+++ b/figure/FFN/FFN.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\astrocyte_neuron\figure\FFN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936A8D5C-2BE9-4944-A3E4-8D0F807C074F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3100755B-CB21-42DF-9065-0FECE8572805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18060" yWindow="2160" windowWidth="23040" windowHeight="12660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="AMPA" sheetId="2" r:id="rId1"/>
+    <sheet name="GABA" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -288,7 +288,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,12 +328,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -402,7 +396,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -685,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9309CA5-B4FD-044A-B7EF-9F9B6F26A726}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="133" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="133" workbookViewId="0">
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -697,11 +690,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
       <c r="E1" s="10" t="s">
         <v>10</v>
       </c>
@@ -733,13 +726,13 @@
       <c r="A3">
         <v>0.1</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
         <v>1</v>
       </c>
       <c r="E3" s="14" t="s">
@@ -756,13 +749,13 @@
       <c r="A4">
         <v>0.2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <v>0.995</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6">
         <v>1</v>
       </c>
       <c r="E4" s="14" t="s">
@@ -779,13 +772,13 @@
       <c r="A5">
         <v>0.3</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="6">
         <v>0.93620000000000003</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>0.96730000000000005</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="14">
         <v>1</v>
       </c>
       <c r="E5" s="19" t="s">
@@ -802,13 +795,13 @@
       <c r="A6">
         <v>0.4</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="6">
         <v>0.8911</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="6">
         <v>0.91759999999999997</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="6">
         <v>0.96050000000000002</v>
       </c>
       <c r="E6" s="19" t="s">
@@ -825,13 +818,13 @@
       <c r="A7">
         <v>0.5</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="6">
         <v>0.86119999999999997</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="6">
         <v>0.90380000000000005</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="6">
         <v>0.93559999999999999</v>
       </c>
       <c r="E7" s="19" t="s">
@@ -848,13 +841,13 @@
       <c r="A8">
         <v>0.6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="6">
         <v>0.85919999999999996</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>0.88180000000000003</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>0.92769999999999997</v>
       </c>
       <c r="E8" s="19" t="s">
@@ -871,13 +864,13 @@
       <c r="A9">
         <v>0.7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="11">
         <v>0.86409999999999998</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>0.8669</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>0.90400000000000003</v>
       </c>
       <c r="E9" s="19" t="s">
@@ -894,13 +887,13 @@
       <c r="A10">
         <v>0.8</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="6">
         <v>0.86299999999999999</v>
       </c>
       <c r="C10" s="11">
         <v>0.87919999999999998</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="6">
         <v>0.89890000000000003</v>
       </c>
       <c r="E10" s="19" t="s">
@@ -917,13 +910,13 @@
       <c r="A11">
         <v>0.9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="6">
         <v>0.86399999999999999</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>0.871</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>0.88800000000000001</v>
       </c>
       <c r="E11" s="19" t="s">
@@ -940,13 +933,13 @@
       <c r="A12">
         <v>1</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="6">
         <v>0.85589999999999999</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>0.86109999999999998</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>0.88080000000000003</v>
       </c>
       <c r="E12" s="19" t="s">
@@ -963,13 +956,13 @@
       <c r="A13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="11">
         <v>0.87619999999999998</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="6">
         <v>0.85450000000000004</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="6">
         <v>0.86529999999999996</v>
       </c>
       <c r="E13" s="13" t="s">
@@ -986,13 +979,13 @@
       <c r="A14">
         <v>1.2</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="6">
         <v>0.88690000000000002</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <v>0.85150000000000003</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="6">
         <v>0.85580000000000001</v>
       </c>
       <c r="E14" s="13" t="s">
@@ -1009,13 +1002,13 @@
       <c r="A15">
         <v>1.3</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="6">
         <v>0.87619999999999998</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="6">
         <v>0.84850000000000003</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="6">
         <v>0.8458</v>
       </c>
       <c r="E15" s="13" t="s">
@@ -1032,19 +1025,19 @@
       <c r="A16">
         <v>1.4</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="6">
         <v>0.871</v>
       </c>
       <c r="C16" s="11">
         <v>0.89410000000000001</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="6">
         <v>0.83889999999999998</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="23" t="s">
         <v>32</v>
       </c>
       <c r="G16" s="20" t="s">
@@ -1055,13 +1048,13 @@
       <c r="A17">
         <v>1.5</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="6">
         <v>0.86629999999999996</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="6">
         <v>0.88</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="6">
         <v>0.83260000000000001</v>
       </c>
       <c r="E17" s="13" t="s">
@@ -1078,13 +1071,13 @@
       <c r="A18">
         <v>1.6</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="6">
         <v>0.86170000000000002</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="6">
         <v>0.86619999999999997</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="6">
         <v>0.82520000000000004</v>
       </c>
       <c r="E18" s="18" t="s">
@@ -1101,13 +1094,13 @@
       <c r="A19">
         <v>1.7</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="6">
         <v>0.85199999999999998</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="6">
         <v>0.85399999999999998</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="6">
         <v>0.80959999999999999</v>
       </c>
       <c r="E19" s="18" t="s">
@@ -1124,13 +1117,13 @@
       <c r="A20">
         <v>1.8</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="6">
         <v>0.83730000000000004</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="6">
         <v>0.83530000000000004</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="6">
         <v>0.80330000000000001</v>
       </c>
       <c r="E20" s="18" t="s">
@@ -1147,13 +1140,13 @@
       <c r="A21">
         <v>2</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="6">
         <v>0.79730000000000001</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="6">
         <v>0.80659999999999998</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="6">
         <v>0.79220000000000002</v>
       </c>
       <c r="E21" s="18" t="s">
@@ -1170,13 +1163,13 @@
       <c r="A22">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="6">
         <v>0.78549999999999998</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="6">
         <v>0.78380000000000005</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="6">
         <v>0.76419999999999999</v>
       </c>
       <c r="E22" s="18" t="s">
@@ -1193,13 +1186,13 @@
       <c r="A23">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="6">
         <v>0.78910000000000002</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="6">
         <v>0.77280000000000004</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="6">
         <v>0.75109999999999999</v>
       </c>
       <c r="E23" s="18" t="s">
@@ -1216,13 +1209,13 @@
       <c r="A24">
         <v>2.4</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="11">
         <v>0.81089999999999995</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="6">
         <v>0.76119999999999999</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="6">
         <v>0.74060000000000004</v>
       </c>
       <c r="E24" s="18" t="s">
@@ -1239,13 +1232,13 @@
       <c r="A25">
         <v>2.5</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="6">
         <v>0.81430000000000002</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="6">
         <v>0.75190000000000001</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="6">
         <v>0.72929999999999995</v>
       </c>
       <c r="E25" s="11" t="s">
@@ -1262,19 +1255,19 @@
       <c r="A26">
         <v>2.6</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B26" s="6">
         <v>0.83050000000000002</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="6">
         <v>0.74099999999999999</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="6">
         <v>1</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="24" t="s">
+      <c r="F26" s="23" t="s">
         <v>35</v>
       </c>
       <c r="G26" s="15" t="s">
@@ -1285,19 +1278,19 @@
       <c r="A27">
         <v>2.8</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="6">
         <v>0.85029999999999994</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="6">
         <v>0.74680000000000002</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="6">
         <v>0.71120000000000005</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="24" t="s">
+      <c r="F27" s="23" t="s">
         <v>35</v>
       </c>
       <c r="G27" s="13" t="s">
@@ -1308,13 +1301,13 @@
       <c r="A28">
         <v>2.9</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28" s="6">
         <v>0.84719999999999995</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="11">
         <v>0.75270000000000004</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="6">
         <v>0.69610000000000005</v>
       </c>
       <c r="E28" s="12" t="s">
@@ -1331,13 +1324,13 @@
       <c r="A29">
         <v>3</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
+      <c r="B29" s="6">
+        <v>1</v>
+      </c>
+      <c r="C29" s="6">
         <v>0.77380000000000004</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="6">
         <v>1</v>
       </c>
       <c r="E29" s="15" t="s">
@@ -1354,13 +1347,13 @@
       <c r="A30">
         <v>3.1</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" s="11">
+      <c r="B30" s="6">
+        <v>1</v>
+      </c>
+      <c r="C30" s="6">
         <v>0.80049999999999999</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="6">
         <v>0.69310000000000005</v>
       </c>
       <c r="E30" s="15" t="s">
@@ -1369,7 +1362,7 @@
       <c r="F30" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="24" t="s">
+      <c r="G30" s="23" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1377,13 +1370,13 @@
       <c r="A31">
         <v>3.2</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="6">
         <v>0.82320000000000004</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="6">
         <v>0.75349999999999995</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="6">
         <v>1</v>
       </c>
       <c r="E31" s="11" t="s">
@@ -1400,13 +1393,13 @@
       <c r="A32">
         <v>3.3</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="6">
         <v>0.81410000000000005</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="6">
         <v>0.78190000000000004</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="6">
         <v>0.70679999999999998</v>
       </c>
       <c r="E32" s="12" t="s">
@@ -1423,13 +1416,13 @@
       <c r="A33">
         <v>3.4</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="6">
         <v>0.80479999999999996</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="6">
         <v>0.77580000000000005</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="6">
         <v>1</v>
       </c>
       <c r="E33" s="11" t="s">
@@ -1446,13 +1439,13 @@
       <c r="A34">
         <v>3.5</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34">
+      <c r="B34" s="6">
+        <v>1</v>
+      </c>
+      <c r="C34" s="6">
         <v>0.79790000000000005</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="6">
         <v>0.71419999999999995</v>
       </c>
       <c r="E34" s="15" t="s">
@@ -1469,13 +1462,13 @@
       <c r="A35">
         <v>3.6</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35">
+      <c r="B35" s="6">
+        <v>1</v>
+      </c>
+      <c r="C35" s="6">
         <v>0.80449999999999999</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35" s="6">
         <v>0.69240000000000002</v>
       </c>
       <c r="E35" s="15" t="s">
@@ -1492,13 +1485,13 @@
       <c r="A36">
         <v>3.7</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="6">
         <v>0.78110000000000002</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="6">
         <v>0.755</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="6">
         <v>0.73170000000000002</v>
       </c>
       <c r="E36" s="12" t="s">
@@ -1515,13 +1508,13 @@
       <c r="A37">
         <v>3.8</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="6">
         <v>0.77790000000000004</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="6">
         <v>0.80289999999999995</v>
       </c>
-      <c r="D37" s="11">
+      <c r="D37" s="6">
         <v>0.71379999999999999</v>
       </c>
       <c r="E37" s="11" t="s">
@@ -1530,7 +1523,7 @@
       <c r="F37" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="G37" s="23" t="s">
+      <c r="G37" s="22" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1538,13 +1531,13 @@
       <c r="A38">
         <v>3.9</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="6">
         <v>0.77490000000000003</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="6">
         <v>0.78149999999999997</v>
       </c>
-      <c r="D38" s="11">
+      <c r="D38" s="6">
         <v>0.70920000000000005</v>
       </c>
       <c r="E38" s="11" t="s">
@@ -1553,7 +1546,7 @@
       <c r="F38" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G38" s="23" t="s">
+      <c r="G38" s="22" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1561,13 +1554,13 @@
       <c r="A39">
         <v>4</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="6">
         <v>0.77159999999999995</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="6">
         <v>0.78810000000000002</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="6">
         <v>0.71250000000000002</v>
       </c>
       <c r="E39" s="11" t="s">
@@ -1584,19 +1577,19 @@
       <c r="A40">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="6">
         <v>0.76670000000000005</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="6">
         <v>0.78039999999999998</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="6">
         <v>0.70350000000000001</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F40" s="23" t="s">
+      <c r="F40" s="22" t="s">
         <v>55</v>
       </c>
       <c r="G40" s="21" t="s">
@@ -1607,13 +1600,13 @@
       <c r="A41">
         <v>4.2</v>
       </c>
-      <c r="B41" s="11">
+      <c r="B41" s="6">
         <v>0.76370000000000005</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="6">
         <v>0.77590000000000003</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="6">
         <v>0.70289999999999997</v>
       </c>
       <c r="E41" s="11" t="s">
@@ -1630,13 +1623,13 @@
       <c r="A42">
         <v>4.3</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="6">
         <v>0.75890000000000002</v>
       </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42">
+      <c r="C42" s="6">
+        <v>1</v>
+      </c>
+      <c r="D42" s="6">
         <v>0.67379999999999995</v>
       </c>
       <c r="E42" s="11" t="s">
@@ -1653,13 +1646,13 @@
       <c r="A43">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="6">
         <v>0.75600000000000001</v>
       </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43" s="11">
+      <c r="C43" s="6">
+        <v>1</v>
+      </c>
+      <c r="D43" s="6">
         <v>0.66969999999999996</v>
       </c>
       <c r="E43" s="11" t="s">
@@ -1676,13 +1669,13 @@
       <c r="A44">
         <v>4.5</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="6">
         <v>0.75249999999999995</v>
       </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44" s="11">
+      <c r="C44" s="6">
+        <v>1</v>
+      </c>
+      <c r="D44" s="6">
         <v>0.71199999999999997</v>
       </c>
       <c r="E44" s="11" t="s">
@@ -1699,13 +1692,13 @@
       <c r="A45">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="6">
         <v>0.75070000000000003</v>
       </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45">
+      <c r="C45" s="6">
+        <v>1</v>
+      </c>
+      <c r="D45" s="6">
         <v>0.7097</v>
       </c>
       <c r="E45" s="11" t="s">
@@ -1732,8 +1725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E13B5C-7F0A-DF4A-90E4-ECDD36DEDEBD}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1762,16 +1755,43 @@
       <c r="A3">
         <v>0.1</v>
       </c>
+      <c r="B3">
+        <v>0.98009999999999997</v>
+      </c>
+      <c r="C3">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.15</v>
       </c>
+      <c r="B4">
+        <v>0.91890000000000005</v>
+      </c>
+      <c r="C4">
+        <v>0.99509999999999998</v>
+      </c>
+      <c r="D4">
+        <v>0.99970000000000003</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.2</v>
       </c>
+      <c r="B5">
+        <v>0.9496</v>
+      </c>
+      <c r="C5">
+        <v>0.99270000000000003</v>
+      </c>
+      <c r="D5">
+        <v>0.99670000000000003</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1781,10 +1801,10 @@
         <v>0.96109999999999995</v>
       </c>
       <c r="C6">
-        <v>0.98340000000000005</v>
+        <v>0.99139999999999995</v>
       </c>
       <c r="D6">
-        <v>0.97009999999999996</v>
+        <v>0.99690000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1792,7 +1812,7 @@
         <v>0.3</v>
       </c>
       <c r="B7">
-        <v>0.94189999999999996</v>
+        <v>0.94069999999999998</v>
       </c>
       <c r="C7">
         <v>0.99270000000000003</v>
@@ -1809,10 +1829,10 @@
         <v>0.91569999999999996</v>
       </c>
       <c r="C8">
-        <v>0.91279999999999994</v>
+        <v>0.99039999999999995</v>
       </c>
       <c r="D8">
-        <v>0.9123</v>
+        <v>0.99390000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1823,10 +1843,10 @@
         <v>0.871</v>
       </c>
       <c r="C9">
-        <v>0.87929999999999997</v>
+        <v>0.97199999999999998</v>
       </c>
       <c r="D9">
-        <v>0.88349999999999995</v>
+        <v>0.99260000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1837,10 +1857,10 @@
         <v>0.80589999999999995</v>
       </c>
       <c r="C10">
-        <v>0.79220000000000002</v>
+        <v>0.91879999999999995</v>
       </c>
       <c r="D10">
-        <v>0.81299999999999994</v>
+        <v>0.98829999999999996</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1854,7 +1874,7 @@
         <v>0.8609</v>
       </c>
       <c r="D11">
-        <v>0.9496</v>
+        <v>0.96030000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1865,15 +1885,16 @@
         <v>0.75049999999999994</v>
       </c>
       <c r="C12">
-        <v>0.72440000000000004</v>
+        <v>0.84799999999999998</v>
       </c>
       <c r="D12">
-        <v>0.69530000000000003</v>
+        <v>0.91049999999999998</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
draw pic of v_ca_ip_i curve for neuron
</commit_message>
<xml_diff>
--- a/figure/FFN/FFN.xlsx
+++ b/figure/FFN/FFN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\astrocyte_neuron\figure\FFN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3100755B-CB21-42DF-9065-0FECE8572805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD905B5-A5A6-4A8B-8ED3-89A9B633B28A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18060" yWindow="2160" windowWidth="23040" windowHeight="12660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4956" yWindow="2868" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMPA" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="58">
   <si>
     <t>纯GABA (p=0)</t>
   </si>
@@ -221,6 +221,10 @@
   </si>
   <si>
     <t>不稳定中心变阴阳螺旋波</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>靶波</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -373,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -401,6 +405,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -678,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9309CA5-B4FD-044A-B7EF-9F9B6F26A726}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView zoomScale="133" workbookViewId="0">
-      <selection sqref="A1:D8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="133" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -942,8 +947,8 @@
       <c r="D12" s="6">
         <v>0.88080000000000003</v>
       </c>
-      <c r="E12" s="19" t="s">
-        <v>28</v>
+      <c r="E12" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="F12" s="19" t="s">
         <v>28</v>
@@ -1723,21 +1728,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E13B5C-7F0A-DF4A-90E4-ECDD36DEDEBD}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
@@ -1751,7 +1756,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.1</v>
       </c>
@@ -1765,7 +1770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.15</v>
       </c>
@@ -1779,7 +1784,7 @@
         <v>0.99970000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.2</v>
       </c>
@@ -1793,7 +1798,7 @@
         <v>0.99670000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.25</v>
       </c>
@@ -1807,7 +1812,7 @@
         <v>0.99690000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.3</v>
       </c>
@@ -1821,7 +1826,7 @@
         <v>0.99550000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.35</v>
       </c>
@@ -1835,7 +1840,7 @@
         <v>0.99390000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.4</v>
       </c>
@@ -1848,8 +1853,11 @@
       <c r="D9">
         <v>0.99260000000000004</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.45</v>
       </c>
@@ -1863,7 +1871,7 @@
         <v>0.98829999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.5</v>
       </c>
@@ -1876,8 +1884,11 @@
       <c r="D11">
         <v>0.96030000000000004</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F11" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.55000000000000004</v>
       </c>
@@ -1889,6 +1900,9 @@
       </c>
       <c r="D12">
         <v>0.91049999999999998</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spikeline draw origin 2.26 HOME
</commit_message>
<xml_diff>
--- a/figure/FFN/FFN.xlsx
+++ b/figure/FFN/FFN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\astrocyte_neuron\figure\FFN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD905B5-A5A6-4A8B-8ED3-89A9B633B28A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AB946B-38F2-4B2C-B97B-6780B21E307B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4956" yWindow="2868" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMPA" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="58">
   <si>
     <t>纯GABA (p=0)</t>
   </si>
@@ -377,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -402,10 +402,16 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -681,30 +687,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9309CA5-B4FD-044A-B7EF-9F9B6F26A726}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="133" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:XFD37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="133" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="6" width="38.21875" customWidth="1"/>
-    <col min="7" max="7" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="7" max="7" width="38.21875" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="10" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="25" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
@@ -717,17 +728,23 @@
       <c r="D2">
         <v>0.3</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2">
+        <v>0.4</v>
+      </c>
+      <c r="F2" s="10">
         <v>0.1</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.2</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.1</v>
       </c>
@@ -740,17 +757,18 @@
       <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>27</v>
-      </c>
+      <c r="E3" s="6"/>
       <c r="F3" s="14" t="s">
         <v>27</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.2</v>
       </c>
@@ -763,17 +781,18 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>27</v>
-      </c>
+      <c r="E4" s="6"/>
       <c r="F4" s="14" t="s">
         <v>27</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.3</v>
       </c>
@@ -786,17 +805,21 @@
       <c r="D5" s="14">
         <v>1</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="E5" s="14"/>
       <c r="F5" s="19" t="s">
         <v>28</v>
       </c>
       <c r="G5" s="19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.4</v>
       </c>
@@ -809,17 +832,21 @@
       <c r="D6" s="6">
         <v>0.96050000000000002</v>
       </c>
-      <c r="E6" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="E6" s="6"/>
       <c r="F6" s="19" t="s">
         <v>28</v>
       </c>
       <c r="G6" s="19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -832,17 +859,21 @@
       <c r="D7" s="6">
         <v>0.93559999999999999</v>
       </c>
-      <c r="E7" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="19" t="s">
         <v>28</v>
       </c>
       <c r="G7" s="19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.6</v>
       </c>
@@ -855,17 +886,21 @@
       <c r="D8" s="6">
         <v>0.92769999999999997</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="E8" s="6"/>
       <c r="F8" s="19" t="s">
         <v>28</v>
       </c>
       <c r="G8" s="19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.7</v>
       </c>
@@ -878,17 +913,21 @@
       <c r="D9" s="6">
         <v>0.90400000000000003</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="E9" s="6"/>
       <c r="F9" s="19" t="s">
         <v>28</v>
       </c>
       <c r="G9" s="19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.8</v>
       </c>
@@ -901,17 +940,21 @@
       <c r="D10" s="6">
         <v>0.89890000000000003</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="E10" s="6"/>
       <c r="F10" s="19" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.9</v>
       </c>
@@ -924,17 +967,21 @@
       <c r="D11" s="6">
         <v>0.88800000000000001</v>
       </c>
-      <c r="E11" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="E11" s="6"/>
       <c r="F11" s="19" t="s">
         <v>28</v>
       </c>
       <c r="G11" s="19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -947,17 +994,21 @@
       <c r="D12" s="6">
         <v>0.88080000000000003</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="6"/>
+      <c r="F12" s="13" t="s">
         <v>9</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>28</v>
       </c>
       <c r="G12" s="19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1.1000000000000001</v>
       </c>
@@ -970,17 +1021,21 @@
       <c r="D13" s="6">
         <v>0.86529999999999996</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="6"/>
+      <c r="F13" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="G13" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="H13" s="20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.2</v>
       </c>
@@ -993,17 +1048,21 @@
       <c r="D14" s="6">
         <v>0.85580000000000001</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="6"/>
+      <c r="F14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="G14" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="H14" s="20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.3</v>
       </c>
@@ -1016,17 +1075,21 @@
       <c r="D15" s="6">
         <v>0.8458</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="6"/>
+      <c r="F15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="G15" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="H15" s="20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1.4</v>
       </c>
@@ -1039,17 +1102,21 @@
       <c r="D16" s="6">
         <v>0.83889999999999998</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="6"/>
+      <c r="F16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="G16" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="H16" s="20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.5</v>
       </c>
@@ -1062,17 +1129,21 @@
       <c r="D17" s="6">
         <v>0.83260000000000001</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="6"/>
+      <c r="F17" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="G17" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="H17" s="20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.6</v>
       </c>
@@ -1085,17 +1156,21 @@
       <c r="D18" s="6">
         <v>0.82520000000000004</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="6"/>
+      <c r="F18" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="G18" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="H18" s="20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.7</v>
       </c>
@@ -1108,17 +1183,21 @@
       <c r="D19" s="6">
         <v>0.80959999999999999</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="6"/>
+      <c r="F19" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="G19" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="H19" s="20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1.8</v>
       </c>
@@ -1131,17 +1210,21 @@
       <c r="D20" s="6">
         <v>0.80330000000000001</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="6"/>
+      <c r="F20" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="G20" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="H20" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1154,17 +1237,21 @@
       <c r="D21" s="6">
         <v>0.79220000000000002</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="6"/>
+      <c r="F21" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>33</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2.2000000000000002</v>
       </c>
@@ -1177,17 +1264,21 @@
       <c r="D22" s="6">
         <v>0.76419999999999999</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="6"/>
+      <c r="F22" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>33</v>
       </c>
       <c r="G22" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2.2999999999999998</v>
       </c>
@@ -1200,17 +1291,21 @@
       <c r="D23" s="6">
         <v>0.75109999999999999</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="6"/>
+      <c r="F23" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>33</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2.4</v>
       </c>
@@ -1223,17 +1318,21 @@
       <c r="D24" s="6">
         <v>0.74060000000000004</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="6"/>
+      <c r="F24" s="18" t="s">
         <v>12</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>33</v>
       </c>
       <c r="G24" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2.5</v>
       </c>
@@ -1246,17 +1345,23 @@
       <c r="D25" s="6">
         <v>0.72929999999999995</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="6">
+        <v>1</v>
+      </c>
+      <c r="F25" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="G25" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="G25" s="13" t="s">
+      <c r="H25" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2.6</v>
       </c>
@@ -1269,17 +1374,23 @@
       <c r="D26" s="6">
         <v>1</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="6">
+        <v>1</v>
+      </c>
+      <c r="F26" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="23" t="s">
+      <c r="G26" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="H26" s="15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2.8</v>
       </c>
@@ -1292,17 +1403,21 @@
       <c r="D27" s="6">
         <v>0.71120000000000005</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="6"/>
+      <c r="F27" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="G27" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="H27" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2.9</v>
       </c>
@@ -1315,17 +1430,23 @@
       <c r="D28" s="6">
         <v>0.69610000000000005</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="6">
+        <v>1</v>
+      </c>
+      <c r="F28" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F28" s="18" t="s">
+      <c r="G28" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="H28" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1338,17 +1459,23 @@
       <c r="D29" s="6">
         <v>1</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="6">
+        <v>1</v>
+      </c>
+      <c r="F29" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F29" s="18" t="s">
+      <c r="G29" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G29" s="15" t="s">
+      <c r="H29" s="15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3.1</v>
       </c>
@@ -1361,17 +1488,23 @@
       <c r="D30" s="6">
         <v>0.69310000000000005</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="6">
+        <v>1</v>
+      </c>
+      <c r="F30" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="18" t="s">
+      <c r="G30" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="23" t="s">
+      <c r="H30" s="23" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3.2</v>
       </c>
@@ -1384,17 +1517,23 @@
       <c r="D31" s="6">
         <v>1</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="6">
+        <v>1</v>
+      </c>
+      <c r="F31" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="G31" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G31" s="15" t="s">
+      <c r="H31" s="15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3.3</v>
       </c>
@@ -1407,17 +1546,23 @@
       <c r="D32" s="6">
         <v>0.70679999999999998</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="6">
+        <v>1</v>
+      </c>
+      <c r="F32" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F32" s="16" t="s">
+      <c r="G32" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="18" t="s">
+      <c r="H32" s="18" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3.4</v>
       </c>
@@ -1430,17 +1575,23 @@
       <c r="D33" s="6">
         <v>1</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="6">
+        <v>1</v>
+      </c>
+      <c r="F33" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="G33" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G33" s="15" t="s">
+      <c r="H33" s="15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3.5</v>
       </c>
@@ -1453,17 +1604,23 @@
       <c r="D34" s="6">
         <v>0.71419999999999995</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="6">
+        <v>1</v>
+      </c>
+      <c r="F34" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="21" t="s">
+      <c r="G34" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="G34" s="16" t="s">
+      <c r="H34" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3.6</v>
       </c>
@@ -1476,17 +1633,23 @@
       <c r="D35" s="6">
         <v>0.69240000000000002</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="6">
+        <v>1</v>
+      </c>
+      <c r="F35" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F35" s="21" t="s">
+      <c r="G35" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="G35" s="16" t="s">
+      <c r="H35" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3.7</v>
       </c>
@@ -1499,17 +1662,23 @@
       <c r="D36" s="6">
         <v>0.73170000000000002</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="6">
+        <v>1</v>
+      </c>
+      <c r="F36" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F36" s="21" t="s">
+      <c r="G36" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="G36" s="17" t="s">
+      <c r="H36" s="17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I36" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3.8</v>
       </c>
@@ -1522,17 +1691,21 @@
       <c r="D37" s="6">
         <v>0.71379999999999999</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="6"/>
+      <c r="F37" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F37" s="21" t="s">
+      <c r="G37" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="G37" s="22" t="s">
+      <c r="H37" s="22" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I37" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3.9</v>
       </c>
@@ -1545,17 +1718,21 @@
       <c r="D38" s="6">
         <v>0.70920000000000005</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E38" s="6"/>
+      <c r="F38" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F38" s="21" t="s">
+      <c r="G38" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G38" s="22" t="s">
+      <c r="H38" s="22" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I38" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4</v>
       </c>
@@ -1568,17 +1745,21 @@
       <c r="D39" s="6">
         <v>0.71250000000000002</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E39" s="6"/>
+      <c r="F39" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F39" s="21" t="s">
+      <c r="G39" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G39" s="11" t="s">
+      <c r="H39" s="11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I39" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4.0999999999999996</v>
       </c>
@@ -1591,17 +1772,21 @@
       <c r="D40" s="6">
         <v>0.70350000000000001</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="E40" s="6"/>
+      <c r="F40" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F40" s="22" t="s">
+      <c r="G40" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="G40" s="21" t="s">
+      <c r="H40" s="21" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I40" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4.2</v>
       </c>
@@ -1614,17 +1799,21 @@
       <c r="D41" s="6">
         <v>0.70289999999999997</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="E41" s="6"/>
+      <c r="F41" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="G41" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="G41" s="12" t="s">
+      <c r="H41" s="12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I41" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>4.3</v>
       </c>
@@ -1637,17 +1826,21 @@
       <c r="D42" s="6">
         <v>0.67379999999999995</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="6"/>
+      <c r="F42" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="G42" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G42" s="12" t="s">
+      <c r="H42" s="12" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I42" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>4.4000000000000004</v>
       </c>
@@ -1660,17 +1853,21 @@
       <c r="D43" s="6">
         <v>0.66969999999999996</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="E43" s="6"/>
+      <c r="F43" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F43" s="15" t="s">
+      <c r="G43" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G43" s="12" t="s">
+      <c r="H43" s="12" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I43" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>4.5</v>
       </c>
@@ -1683,17 +1880,21 @@
       <c r="D44" s="6">
         <v>0.71199999999999997</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="E44" s="6"/>
+      <c r="F44" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="G44" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G44" s="12" t="s">
+      <c r="H44" s="12" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I44" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>4.5999999999999996</v>
       </c>
@@ -1706,20 +1907,21 @@
       <c r="D45" s="6">
         <v>0.7097</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E45" s="6"/>
+      <c r="F45" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F45" s="15" t="s">
+      <c r="G45" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G45" s="12" t="s">
+      <c r="H45" s="12" t="s">
         <v>48</v>
       </c>
+      <c r="I45" s="11" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:D1"/>
-  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1853,7 +2055,7 @@
       <c r="D9">
         <v>0.99260000000000004</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="24" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1884,7 +2086,7 @@
       <c r="D11">
         <v>0.96030000000000004</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="24" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1901,7 +2103,7 @@
       <c r="D12">
         <v>0.91049999999999998</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="G12" s="24" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>